<commit_message>
phu hieu, bang ten
</commit_message>
<xml_diff>
--- a/public/file/mau_excel.xlsx
+++ b/public/file/mau_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnTotNghiep\Github\CaoThangManagementSystem\public\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnTotNghiep\Github\testInPhuHieu\CaoThangManagementSystem\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>ma_sv</t>
   </si>
@@ -32,9 +32,6 @@
     <t>ten_sinh_vien</t>
   </si>
   <si>
-    <t>Lê Đức Moy</t>
-  </si>
-  <si>
     <t>so_dien_thoai</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Sài Gòn</t>
   </si>
   <si>
-    <t>King</t>
-  </si>
-  <si>
     <t>2002/04/04</t>
   </si>
   <si>
@@ -132,6 +126,18 @@
   </si>
   <si>
     <t>HCM</t>
+  </si>
+  <si>
+    <t>Kinh</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>0123456789</t>
   </si>
 </sst>
 </file>
@@ -141,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +156,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -157,15 +172,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -173,21 +200,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,171 +623,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
+    <row r="2" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="2"/>
+      <c r="N4" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>1234</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>2020</v>
+      </c>
+      <c r="M5" t="s">
         <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4">
-        <v>2020</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1 M4:M1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M1048576 M5 L6 M2">
       <formula1>"Cao đẳng ngành,Cao đẳng nghề"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"Nam,Nữ"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>